<commit_message>
update readme to reference old repository
</commit_message>
<xml_diff>
--- a/Data Analysis/Smith Creek Deployment Log.xlsx
+++ b/Data Analysis/Smith Creek Deployment Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bresnahanp/Dropbox/Smart_Coasts_Sensors/Water-Level/Open-Water-Level/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D00F0B-7CBC-8644-A253-99106137FC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8278EFF3-6C45-0944-AF18-C81FEF54CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="3160" windowWidth="38400" windowHeight="21100" xr2:uid="{2C2A2005-0F3A-5045-8878-F39D51731DE6}"/>
+    <workbookView xWindow="-38400" yWindow="2040" windowWidth="38400" windowHeight="21100" xr2:uid="{2C2A2005-0F3A-5045-8878-F39D51731DE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>ft @ Wilmington tide gauge</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>OLD CALCULATIONS; SUPERSEDED BY ANDREA'S RTK POINTS ABOVE</t>
+  </si>
+  <si>
+    <t>N 23rd St</t>
+  </si>
+  <si>
+    <t>N Kerr Ave</t>
   </si>
 </sst>
 </file>
@@ -196,11 +202,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -540,7 +545,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,22 +569,22 @@
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -608,10 +613,10 @@
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="2">
@@ -623,7 +628,7 @@
       <c r="F4" s="2">
         <v>0.32</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1.899</v>
       </c>
       <c r="H4" t="s">
@@ -657,10 +662,10 @@
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="2">
@@ -672,7 +677,7 @@
       <c r="F6" s="2">
         <v>0.15</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>3.5150000000000001</v>
       </c>
       <c r="H6" t="s">
@@ -680,7 +685,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -731,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>A15+A13</f>
         <v>441.06237000000004</v>
@@ -740,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>A16+A13</f>
         <v>281.60818999999998</v>
@@ -749,20 +754,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>